<commit_message>
convert input to array
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>الاسم</t>
   </si>
@@ -48,6 +49,24 @@
   </si>
   <si>
     <t>اي بتنجان</t>
+  </si>
+  <si>
+    <t>الرقم</t>
+  </si>
+  <si>
+    <t>ابو صلاح2</t>
+  </si>
+  <si>
+    <t>لؤي2</t>
+  </si>
+  <si>
+    <t>نبيل2</t>
+  </si>
+  <si>
+    <t>هشام2</t>
+  </si>
+  <si>
+    <t>بورعي2</t>
   </si>
 </sst>
 </file>
@@ -373,64 +392,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make output can have same names
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>الاسم</t>
   </si>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +469,17 @@
       </c>
       <c r="C6">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>